<commit_message>
Updated checkpoint with missing parts
</commit_message>
<xml_diff>
--- a/Diagrama de Gantt.xlsx
+++ b/Diagrama de Gantt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo\Desktop\Universidade\LEI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1ECF9EE0-5616-454E-8E94-0205230656FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBE1B7B-BDD6-4AE3-80DA-ABDCEAFB3B41}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4920" xr2:uid="{A356F5B0-7183-44C6-A6C2-563440F44155}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A356F5B0-7183-44C6-A6C2-563440F44155}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -44,28 +44,13 @@
     <t>Discussão do problema</t>
   </si>
   <si>
-    <t>Implementação do Diagrama de Gantt</t>
-  </si>
-  <si>
     <t>Divisão de tarefas</t>
-  </si>
-  <si>
-    <t>Escolha das contas a associar</t>
-  </si>
-  <si>
-    <t>Revisão do trabalho efetuado</t>
   </si>
   <si>
     <t>Testes finais ao serviço</t>
   </si>
   <si>
     <t>Implementação da associação de contas</t>
-  </si>
-  <si>
-    <t>Desenvolvimento da base de dados</t>
-  </si>
-  <si>
-    <t>Implementação da gravação de dados na base</t>
   </si>
   <si>
     <t>Realização de testes locais</t>
@@ -76,13 +61,28 @@
   <si>
     <t>Preparação da apresentação do Checkpoint 2</t>
   </si>
+  <si>
+    <t>Criação do Diagrama de Gantt</t>
+  </si>
+  <si>
+    <t>Implementação de login local</t>
+  </si>
+  <si>
+    <t>Implementação de servidor OAuth2</t>
+  </si>
+  <si>
+    <t>Melhorias à frontend</t>
+  </si>
+  <si>
+    <t>Revisão do trabalho e preparação de relatório</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-816]d/mmm;@"/>
+    <numFmt numFmtId="164" formatCode="[$-816]d/mmm;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -122,8 +122,8 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -145,7 +145,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -158,7 +158,17 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.25562244176680421"/>
+          <c:y val="4.8557328923335856E-2"/>
+          <c:w val="0.71724809451010696"/>
+          <c:h val="0.9200455019970577"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="stacked"/>
@@ -197,10 +207,10 @@
                   <c:v>Divisão de tarefas</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Implementação do Diagrama de Gantt</c:v>
+                  <c:v>Criação do Diagrama de Gantt</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Escolha das contas a associar</c:v>
+                  <c:v>Implementação de login local</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Implementação da associação de contas</c:v>
@@ -209,10 +219,10 @@
                   <c:v>Preparação da apresentação do Checkpoint 1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Desenvolvimento da base de dados</c:v>
+                  <c:v>Implementação de servidor OAuth2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Implementação da gravação de dados na base</c:v>
+                  <c:v>Melhorias à frontend</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Realização de testes locais</c:v>
@@ -221,7 +231,7 @@
                   <c:v>Preparação da apresentação do Checkpoint 2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Revisão do trabalho efetuado</c:v>
+                  <c:v>Revisão do trabalho e preparação de relatório</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>Testes finais ao serviço</c:v>
@@ -239,25 +249,25 @@
                   <c:v>43509</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43521</c:v>
+                  <c:v>43519</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43525</c:v>
+                  <c:v>43522</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43531</c:v>
+                  <c:v>43524</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43534</c:v>
+                  <c:v>43526</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43544</c:v>
+                  <c:v>43546</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43581</c:v>
+                  <c:v>43551</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43590</c:v>
+                  <c:v>43591</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>43604</c:v>
@@ -266,10 +276,10 @@
                   <c:v>43609</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43617</c:v>
+                  <c:v>43614</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43631</c:v>
+                  <c:v>43628</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -316,10 +326,10 @@
                   <c:v>Divisão de tarefas</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Implementação do Diagrama de Gantt</c:v>
+                  <c:v>Criação do Diagrama de Gantt</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Escolha das contas a associar</c:v>
+                  <c:v>Implementação de login local</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Implementação da associação de contas</c:v>
@@ -328,10 +338,10 @@
                   <c:v>Preparação da apresentação do Checkpoint 1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Desenvolvimento da base de dados</c:v>
+                  <c:v>Implementação de servidor OAuth2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Implementação da gravação de dados na base</c:v>
+                  <c:v>Melhorias à frontend</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Realização de testes locais</c:v>
@@ -340,7 +350,7 @@
                   <c:v>Preparação da apresentação do Checkpoint 2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Revisão do trabalho efetuado</c:v>
+                  <c:v>Revisão do trabalho e preparação de relatório</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>Testes finais ao serviço</c:v>
@@ -361,22 +371,22 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>46</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>5</c:v>
@@ -388,7 +398,7 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -453,7 +463,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="465248104"/>
@@ -513,7 +523,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="465247776"/>
@@ -561,7 +571,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1129,8 +1139,8 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>85726</xdr:rowOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1159,7 +1169,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1457,8 +1467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50F424A8-BD3C-4C5D-9E3D-73EC33E1D6B9}">
   <dimension ref="B2:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1492,10 +1502,10 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="3">
-        <v>43521</v>
+        <v>43519</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -1506,21 +1516,21 @@
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C5" s="3">
-        <v>43525</v>
+        <v>43522</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C6" s="3">
-        <v>43531</v>
+        <v>43524</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -1528,51 +1538,51 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C7" s="3">
-        <v>43534</v>
+        <v>43526</v>
       </c>
       <c r="D7">
-        <v>46</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C8" s="3">
-        <v>43544</v>
+        <v>43546</v>
       </c>
       <c r="D8">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C9" s="3">
-        <v>43581</v>
+        <v>43551</v>
       </c>
       <c r="D9">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C10" s="3">
-        <v>43590</v>
+        <v>43591</v>
       </c>
       <c r="D10">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C11" s="3">
         <v>43604</v>
@@ -1583,7 +1593,7 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C12" s="3">
         <v>43609</v>
@@ -1594,10 +1604,10 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C13" s="3">
-        <v>43617</v>
+        <v>43614</v>
       </c>
       <c r="D13">
         <v>14</v>
@@ -1605,13 +1615,13 @@
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C14" s="3">
-        <v>43631</v>
+        <v>43628</v>
       </c>
       <c r="D14">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>